<commit_message>
Dynamic Trade Interface 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Dynamic Trade Interface - 3020706506/Dynamic Trade Interface - 3020706506.xlsx
+++ b/Data/Dynamic Trade Interface - 3020706506/Dynamic Trade Interface - 3020706506.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Dynamic Trade Interface - 3020706506\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Dynamic Trade Interface - 3020706506\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D7AF7-149C-486E-A150-D6F92DF04A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D128D0-0816-4D02-88B4-3304348AB6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lammergeier</author>
+  </authors>
+  <commentList>
+    <comment ref="D66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-20에 새로 추가된 노드들 (3개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="276">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -88,6 +111,9 @@
     <t>icon</t>
   </si>
   <si>
+    <t>아이콘</t>
+  </si>
+  <si>
     <t>pakageID</t>
   </si>
   <si>
@@ -100,6 +126,9 @@
     <t>A small image of what you are trading.</t>
   </si>
   <si>
+    <t>거래하는 상품의 작은 이미지입니다.</t>
+  </si>
+  <si>
     <t>zeracronius.dynamictradeinterface</t>
   </si>
   <si>
@@ -112,6 +141,9 @@
     <t>Button to open the info window.</t>
   </si>
   <si>
+    <t>버튼을 클릭하여 정보 창을 엽니다.</t>
+  </si>
+  <si>
     <t>modName (folderName)</t>
   </si>
   <si>
@@ -124,6 +156,9 @@
     <t>caption</t>
   </si>
   <si>
+    <t>품목</t>
+  </si>
+  <si>
     <t>Dynamic Trade Interface - 3020706506</t>
   </si>
   <si>
@@ -136,6 +171,9 @@
     <t>Shows the name.</t>
   </si>
   <si>
+    <t>이름을 보여줍니다</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeExtraIconsDef.label</t>
   </si>
   <si>
@@ -145,6 +183,9 @@
     <t>extra icons</t>
   </si>
   <si>
+    <t>추가 아이콘</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeExtraIconsDef.description</t>
   </si>
   <si>
@@ -154,6 +195,9 @@
     <t>Additional icons shown in different situations.</t>
   </si>
   <si>
+    <t>상황에 따라 추가 아이콘이 표시됩니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeQuantityDef.label</t>
   </si>
   <si>
@@ -163,6 +207,9 @@
     <t>available</t>
   </si>
   <si>
+    <t>수량</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeQuantityDef.description</t>
   </si>
   <si>
@@ -172,6 +219,9 @@
     <t>Quantity available for buying or selling.</t>
   </si>
   <si>
+    <t>구매 또는 판매할 수 있는 수량입니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradePriceDef.label</t>
   </si>
   <si>
@@ -181,6 +231,9 @@
     <t>price</t>
   </si>
   <si>
+    <t>가격</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradePriceDef.description</t>
   </si>
   <si>
@@ -190,6 +243,9 @@
     <t>Shows the price.</t>
   </si>
   <si>
+    <t>가격을 보여 줍니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeCounterDef.label</t>
   </si>
   <si>
@@ -199,6 +255,9 @@
     <t>counter box</t>
   </si>
   <si>
+    <t>카운터 박스</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeCounterDef.description</t>
   </si>
   <si>
@@ -208,6 +267,9 @@
     <t>Numeric box where the current quantity bought or sold is shown and can be entered manually.</t>
   </si>
   <si>
+    <t>현재 구매 또는 판매된 수량이 표시되는 입력 박스로, 수동으로 입력할 수 있습니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeButtonsDef.label</t>
   </si>
   <si>
@@ -217,6 +279,9 @@
     <t>buttons</t>
   </si>
   <si>
+    <t>버튼</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeButtonsDef.description</t>
   </si>
   <si>
@@ -226,6 +291,9 @@
     <t>Buttons used to increment or decrement the amount bought or sold.\nClicking the double arrow buttons will increase to most affordable by either party on first click and then to max quantity if clicked again. Hold shift to skip.</t>
   </si>
   <si>
+    <t>구매 또는 판매 금액을 늘리거나 줄이는 데 사용되는 버튼입니다.\n이중 화살표를 한번 클릭하면 살 수 있는 한도 내에서 최대 수량이 선택되며 다시 한번 더 클릭하면 물품의 최대 수량이 선택됩니다. Shift 키를 길게 누르면 건너뛸수 있습니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colDurabilityDef.label</t>
   </si>
   <si>
@@ -235,6 +303,19 @@
     <t>d</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>내구도</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colDurabilityDef.description</t>
   </si>
   <si>
@@ -244,6 +325,9 @@
     <t>Shows the remaining hitpoints (if any) as a percentage.</t>
   </si>
   <si>
+    <t>남은 내구도(있는 경우)를 백분율로 표시합니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colPricePerWeightDef.label</t>
   </si>
   <si>
@@ -262,6 +346,9 @@
     <t>Shows the price divided by mass.</t>
   </si>
   <si>
+    <t>가격을 질량으로 나눈 값을 표시합니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeCounterLabelDef.label</t>
   </si>
   <si>
@@ -277,6 +364,9 @@
     <t>A faster read-only version of the counter box where the current quantity bought or sold is shown.</t>
   </si>
   <si>
+    <t>현재 구매 또는 판매된 수량이 표시되는 카운터 상자의 읽기 전용 버전이 더 빨라졌습니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colCategoryDef.label</t>
   </si>
   <si>
@@ -286,6 +376,9 @@
     <t>category</t>
   </si>
   <si>
+    <t>카테고리</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colCategoryDef.description</t>
   </si>
   <si>
@@ -295,6 +388,9 @@
     <t>Shows the main category of the thing.</t>
   </si>
   <si>
+    <t>항목의 주요 카테고리를 표시합니다.</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTableControlSearchPlaceholder</t>
   </si>
   <si>
@@ -307,6 +403,9 @@
     <t>Search...</t>
   </si>
   <si>
+    <t>검색</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowTitle</t>
   </si>
   <si>
@@ -316,6 +415,9 @@
     <t>Trade window Configuration</t>
   </si>
   <si>
+    <t>거래 창 구성</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowHideUnwilling</t>
   </si>
   <si>
@@ -325,6 +427,9 @@
     <t>Exclude unwilling items</t>
   </si>
   <si>
+    <t>원치 않는 항목 제외</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowHideUnwillingTooltip</t>
   </si>
   <si>
@@ -334,6 +439,9 @@
     <t>Exclude all items trader is unwilling to buy.</t>
   </si>
   <si>
+    <t>상인이 구매하지 않으려는 모든 아이템을 제외합니다.</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowSelectedColumns</t>
   </si>
   <si>
@@ -343,6 +451,9 @@
     <t>Selected columns</t>
   </si>
   <si>
+    <t>추가 되어있는 열</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowAvailableColumns</t>
   </si>
   <si>
@@ -352,6 +463,9 @@
     <t>Available columns</t>
   </si>
   <si>
+    <t>추가 가능한 열</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowEnableProfiling</t>
   </si>
   <si>
@@ -361,6 +475,9 @@
     <t>Enable profiling</t>
   </si>
   <si>
+    <t>프로파일링 사용</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowEnableGhostButtons</t>
   </si>
   <si>
@@ -370,6 +487,9 @@
     <t>Ghost buttons</t>
   </si>
   <si>
+    <t>고스트 버튼</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowEnableGhostButtonsTooltip</t>
   </si>
   <si>
@@ -379,6 +499,9 @@
     <t>Improve performance by only showing trade buttons near the cursor.</t>
   </si>
   <si>
+    <t>마우스 커서 근처에만 버튼을 표시하여 성능을 개선합니다.</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowRememberSortings</t>
   </si>
   <si>
@@ -388,6 +511,9 @@
     <t>Remember sorting</t>
   </si>
   <si>
+    <t>정렬 기억하기</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowRememberSortingsTooltip</t>
   </si>
   <si>
@@ -397,6 +523,9 @@
     <t>Save column sortings in mod configurations.</t>
   </si>
   <si>
+    <t>구성에서 설정한 열 정렬을 저장합니다.</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowResetWidths</t>
   </si>
   <si>
@@ -406,6 +535,9 @@
     <t>Reset widths</t>
   </si>
   <si>
+    <t>너비 초기화</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowEnableBulkDurability</t>
   </si>
   <si>
@@ -415,6 +547,9 @@
     <t>Stacked durability</t>
   </si>
   <si>
+    <t>스택 내구도</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowEnableBulkDurabilityTooltip</t>
   </si>
   <si>
@@ -424,12 +559,31 @@
     <t>Show averaged durability for stacked items in durability column.</t>
   </si>
   <si>
+    <t>내구도 열에 스택된 아이템의 평균 내구도를 표시합니다.</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowAutoRefocus</t>
   </si>
   <si>
     <t>ConfigurationWindowAutoRefocus</t>
   </si>
   <si>
+    <t>자동 재포커스</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Auto refocus</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowAutoRefocusTooltip</t>
   </si>
   <si>
@@ -439,6 +593,9 @@
     <t>Attempts to retain focus on input field when unfocused by changing interface.</t>
   </si>
   <si>
+    <t>인터페이스를 변경하여 포커스가 해제된 경우 입력 필드에 포커스를 유지하려고 시도합니다.</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowColumnDef</t>
   </si>
   <si>
@@ -448,6 +605,9 @@
     <t>Def</t>
   </si>
   <si>
+    <t>정의</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowColumnCaption</t>
   </si>
   <si>
@@ -457,6 +617,9 @@
     <t>Caption</t>
   </si>
   <si>
+    <t>항목</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowColumnAvgMs</t>
   </si>
   <si>
@@ -466,6 +629,9 @@
     <t>Avg ms</t>
   </si>
   <si>
+    <t>평균 ms</t>
+  </si>
+  <si>
     <t>Keyed+ConfigurationWindowColumnMaxMs</t>
   </si>
   <si>
@@ -475,6 +641,9 @@
     <t>Max ms</t>
   </si>
   <si>
+    <t>최대 ms</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowUnwilling</t>
   </si>
   <si>
@@ -484,6 +653,9 @@
     <t>Unwilling</t>
   </si>
   <si>
+    <t>원하지 않음</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowLocked</t>
   </si>
   <si>
@@ -493,6 +665,9 @@
     <t>Window is locked in place.</t>
   </si>
   <si>
+    <t>창이 제자리에 고정되어 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowUnlocked</t>
   </si>
   <si>
@@ -502,6 +677,9 @@
     <t>Window can be dragged.</t>
   </si>
   <si>
+    <t>창을 드래그할 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowGiftLess</t>
   </si>
   <si>
@@ -514,12 +692,51 @@
     <t>Keyed+DynamicTradeWindowGiftNone</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}개 이하 선물.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowGiftNone</t>
   </si>
   <si>
     <t>Keyed+DynamicTradeWindowGiftMore</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gift none.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>선물 안함.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowGiftMore</t>
   </si>
   <si>
@@ -529,6 +746,19 @@
     <t>Keyed+DynamicTradeWindowGiftAll</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}개 이상 선물.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowGiftAll</t>
   </si>
   <si>
@@ -538,6 +768,19 @@
     <t>Keyed+DynamicTradeWindowBuyMore</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>전부 선물.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowBuyMore</t>
   </si>
   <si>
@@ -547,6 +790,19 @@
     <t>Keyed+DynamicTradeWindowBuyAll</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}개 이상 구매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowBuyAll</t>
   </si>
   <si>
@@ -556,6 +812,19 @@
     <t>Keyed+DynamicTradeWindowBuyAffordable</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>전부 구매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowBuyAffordable</t>
   </si>
   <si>
@@ -565,6 +834,19 @@
     <t>Keyed+DynamicTradeWindowSellMore</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>저렴하게 구매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowSellMore</t>
   </si>
   <si>
@@ -574,6 +856,19 @@
     <t>Keyed+DynamicTradeWindowSellAll</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}개 이상 판매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowSellAll</t>
   </si>
   <si>
@@ -583,6 +878,19 @@
     <t>Keyed+DynamicTradeWindowSellAffordable</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>전부 판매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowSellAffordable</t>
   </si>
   <si>
@@ -592,6 +900,19 @@
     <t>Keyed+DynamicTradeWindowUnaffordable</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>저렴하게 판매.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowUnaffordable</t>
   </si>
   <si>
@@ -601,12 +922,28 @@
     <t>Keyed+DynamicTradeWindowGenepackMissing</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>비싸게</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>DynamicTradeWindowGenepackMissing</t>
   </si>
   <si>
     <t>Missing</t>
   </si>
   <si>
+    <t>누락됨</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowGenepackIsolated</t>
   </si>
   <si>
@@ -616,6 +953,9 @@
     <t>Isolated</t>
   </si>
   <si>
+    <t>고립됨</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowGenepackMixed</t>
   </si>
   <si>
@@ -625,6 +965,9 @@
     <t>Mixed</t>
   </si>
   <si>
+    <t>혼합됨</t>
+  </si>
+  <si>
     <t>Keyed+DynamicTradeWindowExtraIconsColumnTrained</t>
   </si>
   <si>
@@ -634,67 +977,55 @@
     <t>Trained</t>
   </si>
   <si>
-    <t>검색</t>
-  </si>
-  <si>
-    <t>거래 창 구성</t>
-  </si>
-  <si>
-    <t>원치 않는 항목 제외</t>
-  </si>
-  <si>
-    <t>상인이 구매하지 않으려는 모든 아이템을 제외합니다.</t>
-  </si>
-  <si>
-    <t>추가 되어있는 열</t>
-  </si>
-  <si>
-    <t>추가 가능한 열</t>
-  </si>
-  <si>
-    <t>프로파일링 사용</t>
-  </si>
-  <si>
-    <t>고스트 버튼</t>
-  </si>
-  <si>
-    <t>마우스 커서 근처에만 버튼을 표시하여 성능을 개선합니다.</t>
-  </si>
-  <si>
-    <t>정의</t>
-  </si>
-  <si>
-    <t>항목</t>
-  </si>
-  <si>
-    <t>평균 ms</t>
-  </si>
-  <si>
-    <t>최대 ms</t>
-  </si>
-  <si>
-    <t>정렬 기억하기</t>
-  </si>
-  <si>
-    <t>구성에서 설정한 열 정렬을 저장합니다.</t>
-  </si>
-  <si>
-    <t>원하지 않음</t>
-  </si>
-  <si>
-    <t>누락됨</t>
-  </si>
-  <si>
-    <t>고립됨</t>
-  </si>
-  <si>
-    <t>혼합됨</t>
-  </si>
-  <si>
-    <t>아이콘</t>
-  </si>
-  <si>
-    <t>거래하는 상품의 작은 이미지입니다.</t>
+    <t>colTradeInfoDef.tooltip</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>훈련됨</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>info button</t>
+  </si>
+  <si>
+    <t>colPricePerWeightDef.tooltip</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>정보 버튼</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>price / kg</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>가격 / kg</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeInfoDef.label</t>
@@ -703,175 +1034,58 @@
     <t>정보 버튼</t>
   </si>
   <si>
-    <t>버튼을 클릭하여 정보 창을 엽니다.</t>
-  </si>
-  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeInfoDef.tooltip</t>
   </si>
   <si>
-    <t>품목</t>
-  </si>
-  <si>
-    <t>이름을 보여줍니다</t>
-  </si>
-  <si>
-    <t>추가 아이콘</t>
-  </si>
-  <si>
-    <t>상황에 따라 추가 아이콘이 표시됩니다.</t>
-  </si>
-  <si>
-    <t>수량</t>
-  </si>
-  <si>
-    <t>구매 또는 판매할 수 있는 수량입니다.</t>
-  </si>
-  <si>
-    <t>가격</t>
-  </si>
-  <si>
-    <t>가격을 보여 줍니다.</t>
-  </si>
-  <si>
-    <t>카운터 박스</t>
-  </si>
-  <si>
-    <t>현재 구매 또는 판매된 수량이 표시되는 입력 박스로, 수동으로 입력할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>현재 구매 또는 판매된 수량이 표시되는 카운터 상자의 읽기 전용 버전이 더 빨라졌습니다.</t>
-  </si>
-  <si>
-    <t>버튼</t>
-  </si>
-  <si>
-    <t>구매 또는 판매 금액을 늘리거나 줄이는 데 사용되는 버튼입니다.\n이중 화살표를 한번 클릭하면 살 수 있는 한도 내에서 최대 수량이 선택되며 다시 한번 더 클릭하면 물품의 최대 수량이 선택됩니다. Shift 키를 길게 누르면 건너뛸수 있습니다.</t>
-  </si>
-  <si>
-    <t>남은 내구도(있는 경우)를 백분율로 표시합니다.</t>
-  </si>
-  <si>
-    <t>가격을 질량으로 나눈 값을 표시합니다.</t>
-  </si>
-  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colPricePerWeightDef.tooltip</t>
   </si>
   <si>
     <t>가격/kg</t>
   </si>
   <si>
-    <t>카테고리</t>
-  </si>
-  <si>
-    <t>항목의 주요 카테고리를 표시합니다.</t>
-  </si>
-  <si>
-    <t>너비 초기화</t>
-  </si>
-  <si>
-    <t>내구도 열에 스택된 아이템의 평균 내구도를 표시합니다.</t>
+    <t>DynamicTradeInterface.Defs.TradeColumnDef+colDurabilityDef.tooltip</t>
+  </si>
+  <si>
+    <t>colDurabilityDef.tooltip</t>
+  </si>
+  <si>
+    <t>Durability</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowOpenAsDefault</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowOpenAsDefault</t>
+  </si>
+  <si>
+    <t>Default trade window</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowOpenAsDefaultTooltip</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowOpenAsDefaultTooltip</t>
+  </si>
+  <si>
+    <t>Use as default trade window. The non-default window can be opened by holding down Ctrl as the window opens.</t>
   </si>
   <si>
     <t>내구도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스택 내구도</t>
-  </si>
-  <si>
-    <t>Auto refocus</t>
+    <t>기본 거래 창</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>인터페이스를 변경하여 포커스가 해제된 경우 입력 필드에 포커스를 유지하려고 시도합니다.</t>
-  </si>
-  <si>
-    <t>자동 재포커스</t>
-  </si>
-  <si>
-    <t>창이 제자리에 고정되어 있습니다.</t>
-  </si>
-  <si>
-    <t>창을 드래그할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>Gift none.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}개 이하 선물.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}개 이상 선물.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>선물 안함.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전부 선물.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}개 이상 구매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전부 구매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>저렴하게 구매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}개 이상 판매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전부 판매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>저렴하게 판매.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비싸게</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>훈련됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>colTradeInfoDef.tooltip</t>
-  </si>
-  <si>
-    <t>colPricePerWeightDef.tooltip</t>
-  </si>
-  <si>
-    <t>info button</t>
-  </si>
-  <si>
-    <t>price / kg</t>
-  </si>
-  <si>
-    <t>정보 버튼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가격 / kg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>기본 거래 창을 사용합니다. 기본 창이 아닌 창은 Ctrl 키를 누른 상태로 열 수 있습니다.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,8 +1100,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,6 +1134,11 @@
         <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -927,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -936,6 +1161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1237,19 +1463,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="2" width="24.75" customWidth="1"/>
     <col min="3" max="3" width="49.25" customWidth="1"/>
     <col min="4" max="4" width="34.25" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="7" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1286,10 +1514,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(A2,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1298,22 +1526,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(A3,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1322,22 +1550,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(A4,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1346,22 +1574,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(A5,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1370,19 +1598,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>218</v>
+        <v>30</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(A6,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1391,19 +1619,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>219</v>
+        <v>34</v>
       </c>
       <c r="G7" t="str">
         <f>VLOOKUP(A7,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1412,19 +1640,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="G8" t="str">
         <f>VLOOKUP(A8,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1433,19 +1661,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>221</v>
+        <v>42</v>
       </c>
       <c r="G9" t="str">
         <f>VLOOKUP(A9,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1454,19 +1682,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>222</v>
+        <v>46</v>
       </c>
       <c r="G10" t="str">
         <f>VLOOKUP(A10,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1475,19 +1703,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>223</v>
+        <v>50</v>
       </c>
       <c r="G11" t="str">
         <f>VLOOKUP(A11,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1496,19 +1724,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>224</v>
+        <v>54</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(A12,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1517,19 +1745,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>225</v>
+        <v>58</v>
       </c>
       <c r="G13" t="str">
         <f>VLOOKUP(A13,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1538,19 +1766,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>226</v>
+        <v>62</v>
       </c>
       <c r="G14" t="str">
         <f>VLOOKUP(A14,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1559,19 +1787,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>228</v>
+        <v>66</v>
       </c>
       <c r="G15" t="str">
         <f>VLOOKUP(A15,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1580,19 +1808,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>229</v>
+        <v>70</v>
       </c>
       <c r="G16" t="str">
         <f>VLOOKUP(A16,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1601,19 +1829,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>238</v>
+        <v>74</v>
       </c>
       <c r="G17" t="str">
         <f>VLOOKUP(A17,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1622,19 +1850,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>230</v>
+        <v>78</v>
       </c>
       <c r="G18" t="str">
         <f>VLOOKUP(A18,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1643,19 +1871,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="G19" t="str">
         <f>VLOOKUP(A19,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1664,19 +1892,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="G20" t="str">
         <f>VLOOKUP(A20,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1685,19 +1913,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>225</v>
+        <v>58</v>
       </c>
       <c r="G21" t="str">
         <f>VLOOKUP(A21,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1706,19 +1934,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>227</v>
+        <v>91</v>
       </c>
       <c r="G22" t="str">
         <f>VLOOKUP(A22,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1727,19 +1955,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>234</v>
+        <v>95</v>
       </c>
       <c r="G23" t="str">
         <f>VLOOKUP(A23,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1748,19 +1976,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>235</v>
+        <v>99</v>
       </c>
       <c r="G24" t="str">
         <f>VLOOKUP(A24,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1769,19 +1997,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="G25" t="str">
         <f>VLOOKUP(A25,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1790,19 +2018,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="G26" t="str">
         <f>VLOOKUP(A26,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1811,19 +2039,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="G27" t="str">
         <f>VLOOKUP(A27,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1832,19 +2060,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
       <c r="G28" t="str">
         <f>VLOOKUP(A28,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1853,19 +2081,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="G29" t="str">
         <f>VLOOKUP(A29,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1874,19 +2102,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="G30" t="str">
         <f>VLOOKUP(A30,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1895,19 +2123,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="G31" t="str">
         <f>VLOOKUP(A31,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1916,19 +2144,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="G32" t="str">
         <f>VLOOKUP(A32,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1937,19 +2165,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="G33" t="str">
         <f>VLOOKUP(A33,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1958,19 +2186,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>205</v>
+        <v>140</v>
       </c>
       <c r="G34" t="str">
         <f>VLOOKUP(A34,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -1979,19 +2207,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="G35" t="str">
         <f>VLOOKUP(A35,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2000,19 +2228,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="G36" t="e">
         <f>VLOOKUP(A36,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2021,19 +2249,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>239</v>
+        <v>152</v>
       </c>
       <c r="G37" t="e">
         <f>VLOOKUP(A37,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2042,19 +2270,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>237</v>
+        <v>156</v>
       </c>
       <c r="G38" t="e">
         <f>VLOOKUP(A38,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2063,19 +2291,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
       <c r="G39" t="e">
         <f>VLOOKUP(A39,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2084,19 +2312,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>241</v>
+        <v>164</v>
       </c>
       <c r="G40" t="e">
         <f>VLOOKUP(A40,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2105,19 +2333,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
       <c r="G41" t="str">
         <f>VLOOKUP(A41,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2126,19 +2354,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="G42" t="str">
         <f>VLOOKUP(A42,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2147,19 +2375,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="G43" t="str">
         <f>VLOOKUP(A43,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2168,19 +2396,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="G44" t="str">
         <f>VLOOKUP(A44,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2189,19 +2417,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="G45" t="str">
         <f>VLOOKUP(A45,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2210,19 +2438,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="G46" t="e">
         <f>VLOOKUP(A46,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2231,19 +2459,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="G47" t="e">
         <f>VLOOKUP(A47,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2252,19 +2480,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="G48" t="e">
         <f>VLOOKUP(A48,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2273,19 +2501,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="G49" t="e">
         <f>VLOOKUP(A49,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2294,19 +2522,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="G50" t="e">
         <f>VLOOKUP(A50,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2315,19 +2543,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="G51" t="e">
         <f>VLOOKUP(A51,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2336,19 +2564,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>250</v>
+        <v>213</v>
       </c>
       <c r="G52" t="e">
         <f>VLOOKUP(A52,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2357,19 +2585,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>163</v>
+        <v>214</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="G53" t="e">
         <f>VLOOKUP(A53,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2378,19 +2606,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="G54" t="e">
         <f>VLOOKUP(A54,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2399,19 +2627,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="G55" t="e">
         <f>VLOOKUP(A55,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2420,19 +2648,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>172</v>
+        <v>226</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="G56" t="e">
         <f>VLOOKUP(A56,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2441,19 +2669,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>175</v>
+        <v>230</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="G57" t="e">
         <f>VLOOKUP(A57,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2462,19 +2690,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>178</v>
+        <v>234</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="G58" t="e">
         <f>VLOOKUP(A58,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2483,19 +2711,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="G59" t="str">
         <f>VLOOKUP(A59,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2504,19 +2732,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>184</v>
+        <v>242</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="G60" t="str">
         <f>VLOOKUP(A60,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2525,19 +2753,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>187</v>
+        <v>246</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="G61" t="str">
         <f>VLOOKUP(A61,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2546,19 +2774,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>189</v>
+        <v>249</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="E62" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G62" t="e">
         <f>VLOOKUP(A62,Sheet1!$A$1:$B$5832,2,FALSE)</f>
@@ -2570,13 +2798,13 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -2584,18 +2812,70 @@
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>264</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>265</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>267</v>
+      </c>
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" t="s">
+        <v>269</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>270</v>
+      </c>
+      <c r="B68" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68" t="s">
+        <v>271</v>
+      </c>
+      <c r="D68" t="s">
+        <v>272</v>
+      </c>
+      <c r="E68" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2611,10 +2891,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>192</v>
+        <v>104</v>
       </c>
       <c r="C1" t="str" cm="1">
         <f t="array" ref="C1">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A1,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2623,10 +2903,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" ref="C2">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A2,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2635,10 +2915,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" ref="C3">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A3,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2647,10 +2927,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A4,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2659,10 +2939,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" ref="C5">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A5,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2671,10 +2951,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" ref="C6">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A6,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2683,10 +2963,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A7,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2695,10 +2975,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" ref="C8">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A8,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2707,10 +2987,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A9,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2719,10 +2999,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A10,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2731,10 +3011,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" ref="C11">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A11,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2743,10 +3023,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" ref="C12">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A12,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2755,10 +3035,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" ref="C13">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A13,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2767,10 +3047,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>205</v>
+        <v>140</v>
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A14,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2779,10 +3059,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" ref="C15">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A15,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2791,10 +3071,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A16,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2803,10 +3083,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A17,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2815,10 +3095,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A18,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2827,10 +3107,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A19,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2842,7 +3122,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" ref="C20">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A20,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2851,10 +3131,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A21,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2863,10 +3143,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>213</v>
+        <v>259</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A22,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2875,10 +3155,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="C23" t="str" cm="1">
         <f t="array" ref="C23">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A23,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2887,10 +3167,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="C24" t="str" cm="1">
         <f t="array" ref="C24">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A24,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2899,10 +3179,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="C25" t="str" cm="1">
         <f t="array" ref="C25">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A25,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2911,10 +3191,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>218</v>
+        <v>30</v>
       </c>
       <c r="C26" t="str" cm="1">
         <f t="array" ref="C26">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A26,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2923,10 +3203,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>219</v>
+        <v>34</v>
       </c>
       <c r="C27" t="str" cm="1">
         <f t="array" ref="C27">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A27,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2935,10 +3215,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="C28" t="str" cm="1">
         <f t="array" ref="C28">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A28,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2947,10 +3227,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>221</v>
+        <v>42</v>
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A29,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2959,10 +3239,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>222</v>
+        <v>46</v>
       </c>
       <c r="C30" t="str" cm="1">
         <f t="array" ref="C30">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A30,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2971,10 +3251,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>223</v>
+        <v>50</v>
       </c>
       <c r="C31" t="str" cm="1">
         <f t="array" ref="C31">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A31,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2983,10 +3263,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>224</v>
+        <v>54</v>
       </c>
       <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A32,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -2995,10 +3275,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>225</v>
+        <v>58</v>
       </c>
       <c r="C33" t="str" cm="1">
         <f t="array" ref="C33">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A33,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3007,10 +3287,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>226</v>
+        <v>62</v>
       </c>
       <c r="C34" t="str" cm="1">
         <f t="array" ref="C34">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A34,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3019,10 +3299,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>225</v>
+        <v>58</v>
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A35,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3031,10 +3311,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>227</v>
+        <v>91</v>
       </c>
       <c r="C36" t="str" cm="1">
         <f t="array" ref="C36">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A36,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3043,10 +3323,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>228</v>
+        <v>66</v>
       </c>
       <c r="C37" t="str" cm="1">
         <f t="array" ref="C37">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A37,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3055,10 +3335,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>229</v>
+        <v>70</v>
       </c>
       <c r="C38" t="str" cm="1">
         <f t="array" ref="C38">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A38,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3067,10 +3347,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C39" t="str" cm="1">
         <f t="array" ref="C39">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A39,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3079,10 +3359,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>230</v>
+        <v>78</v>
       </c>
       <c r="C40" t="str" cm="1">
         <f t="array" ref="C40">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A40,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3091,10 +3371,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C41" t="str" cm="1">
         <f t="array" ref="C41">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A41,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3103,10 +3383,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="C42" t="str" cm="1">
         <f t="array" ref="C42">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A42,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3115,10 +3395,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="C43" t="str" cm="1">
         <f t="array" ref="C43">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A43,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3127,10 +3407,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>234</v>
+        <v>95</v>
       </c>
       <c r="C44" t="str" cm="1">
         <f t="array" ref="C44">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A44,Sheet!$A$2:$A$8004,1,FALSE))</f>
@@ -3139,10 +3419,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>235</v>
+        <v>99</v>
       </c>
       <c r="C45" t="str" cm="1">
         <f t="array" ref="C45">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A45,Sheet!$A$2:$A$8004,1,FALSE))</f>

</xml_diff>

<commit_message>
Dynamic Trade Interface - 3020706506 업데이트
</commit_message>
<xml_diff>
--- a/Data/Dynamic Trade Interface - 3020706506/Dynamic Trade Interface - 3020706506.xlsx
+++ b/Data/Dynamic Trade Interface - 3020706506/Dynamic Trade Interface - 3020706506.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Dynamic Trade Interface - 3020706506\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Dynamic Trade Interface - 3020706506\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9961215D-1A03-49AD-B6A3-40DAC9C1E48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA8B884-768C-483C-82A2-0F2A65140613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,11 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>bjmi0</author>
     <author>Lammergeier</author>
   </authors>
   <commentList>
-    <comment ref="D66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,11 +49,171 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>2024-04-20에 새로 추가된 노드들 (3개)</t>
+          <t>2025-08-08 이전의 원문: 'counter box'</t>
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-08 이전의 원문: 'counter box'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D59" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-08 이전의 원문: 'Missing'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D60" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-08 이전의 원문: 'Isolated'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-08 이전의 원문: 'Mixed'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D66" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-20</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>추가된</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>노드들</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>개</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D69" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -65,12 +226,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="D71" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-08에 새로 추가된 노드들 (22개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -92,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="374">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -265,7 +439,7 @@
     <t>colTradeCounterDef.label</t>
   </si>
   <si>
-    <t>counter box</t>
+    <t>Genepack not owned.</t>
   </si>
   <si>
     <t>카운터 박스</t>
@@ -948,10 +1122,7 @@
     <t>Keyed+DynamicTradeWindowGenepackMissing</t>
   </si>
   <si>
-    <t>DynamicTradeWindowGenepackMissing</t>
-  </si>
-  <si>
-    <t>Missing</t>
+    <t>Genepack owned in isolated pack.</t>
   </si>
   <si>
     <t>누락됨</t>
@@ -963,7 +1134,7 @@
     <t>DynamicTradeWindowGenepackIsolated</t>
   </si>
   <si>
-    <t>Isolated</t>
+    <t>Genepack owned in mixed pack.</t>
   </si>
   <si>
     <t>고립됨</t>
@@ -975,7 +1146,7 @@
     <t>DynamicTradeWindowGenepackMixed</t>
   </si>
   <si>
-    <t>Mixed</t>
+    <t>Keyed+ConfigurationWindowShowAvailableOnMap</t>
   </si>
   <si>
     <t>혼합됨</t>
@@ -1050,16 +1221,13 @@
     <t>Durability</t>
   </si>
   <si>
+    <t>Keyed+ConfigurationWindowOpenAsDefault</t>
+  </si>
+  <si>
     <t>ConfigurationWindowOpenAsDefault</t>
   </si>
   <si>
-    <t>Keyed+ConfigurationWindowOpenAsDefault</t>
-  </si>
-  <si>
     <t>Default trade window</t>
-  </si>
-  <si>
-    <t>Keyed+ConfigurationWindowOpenAsDefaultTooltip</t>
   </si>
   <si>
     <r>
@@ -1075,6 +1243,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+ConfigurationWindowOpenAsDefaultTooltip</t>
+  </si>
+  <si>
     <t>ConfigurationWindowOpenAsDefaultTooltip</t>
   </si>
   <si>
@@ -1084,6 +1255,30 @@
     <t>기본 거래 창을 사용합니다. 기본 창이 아닌 창은 Ctrl 키를 누른 상태로 열 수 있습니다.</t>
   </si>
   <si>
+    <t>Keyed+ConfigurationWindowPauseAfterTrade</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowPauseAfterTrade</t>
+  </si>
+  <si>
+    <t>Pause after trade</t>
+  </si>
+  <si>
+    <t>거래 후 일시정지</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowPauseAfterTradeTooltip</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowPauseAfterTradeTooltip</t>
+  </si>
+  <si>
+    <t>Keeps the game paused after trade window is closed.</t>
+  </si>
+  <si>
+    <t>거래 창이 닫힌 후에도 게임을 일시 정지 상태로 유지합니다.</t>
+  </si>
+  <si>
     <t>DynamicTradeInterface.Defs.TradeColumnDef+colTradeInfoDef.label</t>
   </si>
   <si>
@@ -1099,35 +1294,296 @@
     <t>가격/kg</t>
   </si>
   <si>
-    <t>Keyed+ConfigurationWindowPauseAfterTrade</t>
-  </si>
-  <si>
-    <t>ConfigurationWindowPauseAfterTrade</t>
-  </si>
-  <si>
-    <t>Pause after trade</t>
-  </si>
-  <si>
-    <t>Keyed+ConfigurationWindowPauseAfterTradeTooltip</t>
-  </si>
-  <si>
-    <t>ConfigurationWindowPauseAfterTradeTooltip</t>
-  </si>
-  <si>
-    <t>Keeps the game paused after trade window is closed.</t>
-  </si>
-  <si>
-    <t>거래 창이 닫힌 후에도 게임을 일시 정지 상태로 유지합니다.</t>
-  </si>
-  <si>
-    <t>거래 후 일시정지</t>
+    <t>trading</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowShowAvailableOnMap</t>
+  </si>
+  <si>
+    <t>Show available on map.</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowShowAvailableOnMapTooltip</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowShowAvailableOnMapTooltip</t>
+  </si>
+  <si>
+    <t>Show total available on map if different from what is available for trade in Available column.</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowAlternatingRowColors</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowAlternatingRowColors</t>
+  </si>
+  <si>
+    <t>Row colors.</t>
+  </si>
+  <si>
+    <t>Keyed+ConfigurationWindowAlternatingRowColorsTooltip</t>
+  </si>
+  <si>
+    <t>ConfigurationWindowAlternatingRowColorsTooltip</t>
+  </si>
+  <si>
+    <t>Enable to have a slightly alternating background color per row.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSaveAsPreset</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSaveAsPreset</t>
+  </si>
+  <si>
+    <t>Save filter as preset.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationBell</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationBell</t>
+  </si>
+  <si>
+    <t>Found matches, click to show.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSummaryShow</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSummaryShow</t>
+  </si>
+  <si>
+    <t>Show summary</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSummaryHide</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSummaryHide</t>
+  </si>
+  <si>
+    <t>Hide summary</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSummaryGifting</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSummaryGifting</t>
+  </si>
+  <si>
+    <t>Gifting</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSummaryBuying</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSummaryBuying</t>
+  </si>
+  <si>
+    <t>Buying ({0} {1})</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowSummarySelling</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowSummarySelling</t>
+  </si>
+  <si>
+    <t>Selling ({0} {1})</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsTooltip</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsTooltip</t>
+  </si>
+  <si>
+    <t>Filter presets</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsTitle</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsTitle</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsScopeFilter</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsScopeFilter</t>
+  </si>
+  <si>
+    <t>Click to apply filter.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsEnable</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsEnable</t>
+  </si>
+  <si>
+    <t>Enable notifications.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsAdd</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsAdd</t>
+  </si>
+  <si>
+    <t>Add new preset.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowNotificationsDelete</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowNotificationsDelete</t>
+  </si>
+  <si>
+    <t>Delete preset.</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowColumnContextSortByAscending</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowColumnContextSortByAscending</t>
+  </si>
+  <si>
+    <t>Sort by Ascending</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowColumnContextSortByDescending</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowColumnContextSortByDescending</t>
+  </si>
+  <si>
+    <t>Sort by Descending</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowColumnContextClearSorting</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowColumnContextClearSorting</t>
+  </si>
+  <si>
+    <t>Clear sorting</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowColumnContextHideColumn</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowColumnContextHideColumn</t>
+  </si>
+  <si>
+    <t>Keyed+DynamicTradeWindowColumnContextShowHiddenColumns</t>
+  </si>
+  <si>
+    <t>DynamicTradeWindowColumnContextShowHiddenColumns</t>
+  </si>
+  <si>
+    <t>Show hidden columns:</t>
+  </si>
+  <si>
+    <t>거래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격을 보여줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도 상의 보유량 표시</t>
+  </si>
+  <si>
+    <t>'보유량' 열의 수치와 지도 상의 총 보유량이 다를 경우, 총 보유량도 함께 표시</t>
+  </si>
+  <si>
+    <t>행 색상</t>
+  </si>
+  <si>
+    <t>활성화하면 각 행마다 배경색이 번갈아 표시됩니다.</t>
+  </si>
+  <si>
+    <t>필터를 프리셋으로 저장</t>
+  </si>
+  <si>
+    <t>일치하는 항목 발견, 클릭하여 표시</t>
+  </si>
+  <si>
+    <t>요약 보기</t>
+  </si>
+  <si>
+    <t>요약 숨기기</t>
+  </si>
+  <si>
+    <t>선물하기</t>
+  </si>
+  <si>
+    <t>필터 프리셋</t>
+  </si>
+  <si>
+    <t>클릭하여 필터 적용</t>
+  </si>
+  <si>
+    <t>알림 활성화</t>
+  </si>
+  <si>
+    <t>새 프리셋 추가</t>
+  </si>
+  <si>
+    <t>프리셋 삭제</t>
+  </si>
+  <si>
+    <t>오름차순 정렬</t>
+  </si>
+  <si>
+    <t>내림차순 정렬</t>
+  </si>
+  <si>
+    <t>정렬 초기화</t>
+  </si>
+  <si>
+    <t>열 숨기기</t>
+  </si>
+  <si>
+    <t>숨겨진 열 표시:</t>
+  </si>
+  <si>
+    <t>Hide column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>({0} {1}) 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>({0} {1}) 판매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DynamicTradeWindowGenepackMissing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유전자 미보유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단일 유전자묶음 보유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혼합 유전자묶음 보유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,8 +1604,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,6 +1644,11 @@
         <fgColor rgb="FF87CEEB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1194,7 +1662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1204,6 +1672,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1506,23 +1975,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="9.08203125" customWidth="1"/>
     <col min="2" max="2" width="24.75" customWidth="1"/>
     <col min="3" max="3" width="49.25" customWidth="1"/>
     <col min="4" max="4" width="34.25" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
-    <col min="6" max="7" width="9.125" customWidth="1"/>
+    <col min="6" max="7" width="9.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +2011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1566,7 +2035,7 @@
         <v>아이콘</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1590,7 +2059,7 @@
         <v>거래하는 상품의 작은 이미지입니다.</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +2083,7 @@
         <v>버튼을 클릭하여 정보 창을 엽니다.</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +2107,7 @@
         <v>품목</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1659,7 +2128,7 @@
         <v>이름을 보여줍니다</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +2149,7 @@
         <v>추가 아이콘</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1701,7 +2170,7 @@
         <v>상황에 따라 추가 아이콘이 표시됩니다.</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1722,7 +2191,7 @@
         <v>수량</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -1743,7 +2212,7 @@
         <v>구매 또는 판매할 수 있는 수량입니다.</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1764,7 +2233,7 @@
         <v>가격</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1778,14 +2247,14 @@
         <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>347</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(A12,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>가격을 보여 줍니다.</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
@@ -1795,18 +2264,18 @@
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>57</v>
+      <c r="D13" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>346</v>
       </c>
       <c r="G13" t="str">
         <f>VLOOKUP(A13,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>카운터 박스</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1827,7 +2296,7 @@
         <v>현재 구매 또는 판매된 수량이 표시되는 입력 박스로, 수동으로 입력할 수 있습니다.</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -1848,7 +2317,7 @@
         <v>버튼</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
@@ -1869,7 +2338,7 @@
         <v>구매 또는 판매 금액을 늘리거나 줄이는 데 사용되는 버튼입니다.\n이중 화살표를 한번 클릭하면 살 수 있는 한도 내에서 최대 수량이 선택되며 다시 한번 더 클릭하면 물품의 최대 수량이 선택됩니다. Shift 키를 길게 누르면 건너뛸수 있습니다.</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
@@ -1890,7 +2359,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>75</v>
       </c>
@@ -1911,7 +2380,7 @@
         <v>남은 내구도(있는 경우)를 백분율로 표시합니다.</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -1932,7 +2401,7 @@
         <v>/kg</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1953,7 +2422,7 @@
         <v>가격을 질량으로 나눈 값을 표시합니다.</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>86</v>
       </c>
@@ -1963,18 +2432,18 @@
       <c r="C21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>57</v>
+      <c r="D21" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>346</v>
       </c>
       <c r="G21" t="str">
         <f>VLOOKUP(A21,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>카운터 박스</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>88</v>
       </c>
@@ -1995,7 +2464,7 @@
         <v>현재 구매 또는 판매된 수량이 표시되는 카운터 상자의 읽기 전용 버전이 더 빨라졌습니다.</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
@@ -2016,7 +2485,7 @@
         <v>카테고리</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
@@ -2037,7 +2506,7 @@
         <v>항목의 주요 카테고리를 표시합니다.</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -2058,7 +2527,7 @@
         <v>검색</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>105</v>
       </c>
@@ -2079,7 +2548,7 @@
         <v>거래 창 구성</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>109</v>
       </c>
@@ -2100,7 +2569,7 @@
         <v>원치 않는 항목 제외</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
@@ -2121,7 +2590,7 @@
         <v>상인이 구매하지 않으려는 모든 아이템을 제외합니다.</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>117</v>
       </c>
@@ -2142,7 +2611,7 @@
         <v>추가 되어있는 열</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>121</v>
       </c>
@@ -2163,7 +2632,7 @@
         <v>추가 가능한 열</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>125</v>
       </c>
@@ -2184,7 +2653,7 @@
         <v>프로파일링 사용</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>129</v>
       </c>
@@ -2205,7 +2674,7 @@
         <v>고스트 버튼</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>133</v>
       </c>
@@ -2226,7 +2695,7 @@
         <v>마우스 커서 근처에만 버튼을 표시하여 성능을 개선합니다.</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>137</v>
       </c>
@@ -2247,7 +2716,7 @@
         <v>정렬 기억하기</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>141</v>
       </c>
@@ -2268,7 +2737,7 @@
         <v>구성에서 설정한 열 정렬을 저장합니다.</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>145</v>
       </c>
@@ -2289,7 +2758,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>149</v>
       </c>
@@ -2310,7 +2779,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>153</v>
       </c>
@@ -2331,7 +2800,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>157</v>
       </c>
@@ -2352,7 +2821,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>161</v>
       </c>
@@ -2373,7 +2842,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>165</v>
       </c>
@@ -2394,7 +2863,7 @@
         <v>정의</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -2415,7 +2884,7 @@
         <v>항목</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -2436,7 +2905,7 @@
         <v>평균 ms</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>177</v>
       </c>
@@ -2457,7 +2926,7 @@
         <v>최대 ms</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>181</v>
       </c>
@@ -2478,7 +2947,7 @@
         <v>원하지 않음</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>185</v>
       </c>
@@ -2499,7 +2968,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
@@ -2520,7 +2989,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>193</v>
       </c>
@@ -2541,7 +3010,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>197</v>
       </c>
@@ -2562,7 +3031,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>201</v>
       </c>
@@ -2583,7 +3052,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>205</v>
       </c>
@@ -2604,7 +3073,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>209</v>
       </c>
@@ -2625,7 +3094,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>213</v>
       </c>
@@ -2646,7 +3115,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>217</v>
       </c>
@@ -2667,7 +3136,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>221</v>
       </c>
@@ -2688,7 +3157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>225</v>
       </c>
@@ -2709,7 +3178,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>229</v>
       </c>
@@ -2730,7 +3199,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>233</v>
       </c>
@@ -2751,7 +3220,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>237</v>
       </c>
@@ -2759,130 +3228,130 @@
         <v>101</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>239</v>
+        <v>370</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>240</v>
+        <v>371</v>
       </c>
       <c r="G59" t="str">
         <f>VLOOKUP(A59,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>누락됨</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>243</v>
+      <c r="D60" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>244</v>
+        <v>372</v>
       </c>
       <c r="G60" t="str">
         <f>VLOOKUP(A60,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>고립됨</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>247</v>
+      <c r="D61" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>248</v>
+        <v>373</v>
       </c>
       <c r="G61" t="str">
         <f>VLOOKUP(A61,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>혼합됨</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" t="s">
         <v>251</v>
-      </c>
-      <c r="E62" t="s">
-        <v>252</v>
       </c>
       <c r="G62" t="e">
         <f>VLOOKUP(A62,Sheet1!$A$1:$B$5832,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63" t="s">
         <v>253</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C64" t="s">
+        <v>255</v>
+      </c>
+      <c r="D64" t="s">
         <v>256</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E64" s="1" t="s">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>259</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
       <c r="C66" t="s">
+        <v>259</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B67" t="s">
         <v>101</v>
@@ -2891,13 +3360,13 @@
         <v>262</v>
       </c>
       <c r="D67" t="s">
+        <v>263</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>265</v>
       </c>
@@ -2905,47 +3374,421 @@
         <v>101</v>
       </c>
       <c r="C68" t="s">
+        <v>266</v>
+      </c>
+      <c r="D68" t="s">
         <v>267</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>268</v>
       </c>
-      <c r="E68" t="s">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" t="s">
+        <v>270</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E69" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>273</v>
+      </c>
+      <c r="B70" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" t="s">
+        <v>274</v>
+      </c>
+      <c r="D70" t="s">
         <v>275</v>
       </c>
-      <c r="B69" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="E70" t="s">
         <v>276</v>
       </c>
-      <c r="D69" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="E69" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>278</v>
-      </c>
-      <c r="B70" t="s">
-        <v>101</v>
-      </c>
-      <c r="C70" t="s">
-        <v>279</v>
-      </c>
-      <c r="D70" t="s">
-        <v>280</v>
-      </c>
-      <c r="E70" t="s">
-        <v>281</v>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71" t="s">
+        <v>283</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E71" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>285</v>
+      </c>
+      <c r="B72" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" t="s">
+        <v>286</v>
+      </c>
+      <c r="D72" t="s">
+        <v>287</v>
+      </c>
+      <c r="E72" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>288</v>
+      </c>
+      <c r="B73" t="s">
+        <v>101</v>
+      </c>
+      <c r="C73" t="s">
+        <v>289</v>
+      </c>
+      <c r="D73" t="s">
+        <v>290</v>
+      </c>
+      <c r="E73" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" t="s">
+        <v>292</v>
+      </c>
+      <c r="D74" t="s">
+        <v>293</v>
+      </c>
+      <c r="E74" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" t="s">
+        <v>295</v>
+      </c>
+      <c r="D75" t="s">
+        <v>296</v>
+      </c>
+      <c r="E75" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>297</v>
+      </c>
+      <c r="B76" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" t="s">
+        <v>299</v>
+      </c>
+      <c r="E76" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>300</v>
+      </c>
+      <c r="B77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" t="s">
+        <v>302</v>
+      </c>
+      <c r="E77" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>303</v>
+      </c>
+      <c r="B78" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" t="s">
+        <v>304</v>
+      </c>
+      <c r="D78" t="s">
+        <v>305</v>
+      </c>
+      <c r="E78" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>306</v>
+      </c>
+      <c r="B79" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" t="s">
+        <v>307</v>
+      </c>
+      <c r="D79" t="s">
+        <v>308</v>
+      </c>
+      <c r="E79" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>309</v>
+      </c>
+      <c r="B80" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" t="s">
+        <v>310</v>
+      </c>
+      <c r="D80" t="s">
+        <v>311</v>
+      </c>
+      <c r="E80" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>312</v>
+      </c>
+      <c r="B81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" t="s">
+        <v>313</v>
+      </c>
+      <c r="D81" t="s">
+        <v>314</v>
+      </c>
+      <c r="E81" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>315</v>
+      </c>
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82" t="s">
+        <v>316</v>
+      </c>
+      <c r="D82" t="s">
+        <v>317</v>
+      </c>
+      <c r="E82" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>318</v>
+      </c>
+      <c r="B83" t="s">
+        <v>101</v>
+      </c>
+      <c r="C83" t="s">
+        <v>319</v>
+      </c>
+      <c r="D83" t="s">
+        <v>317</v>
+      </c>
+      <c r="E83" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>320</v>
+      </c>
+      <c r="B84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" t="s">
+        <v>321</v>
+      </c>
+      <c r="D84" t="s">
+        <v>322</v>
+      </c>
+      <c r="E84" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>323</v>
+      </c>
+      <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" t="s">
+        <v>324</v>
+      </c>
+      <c r="D85" t="s">
+        <v>325</v>
+      </c>
+      <c r="E85" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>326</v>
+      </c>
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>329</v>
+      </c>
+      <c r="B87" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" t="s">
+        <v>330</v>
+      </c>
+      <c r="D87" t="s">
+        <v>331</v>
+      </c>
+      <c r="E87" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>332</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" t="s">
+        <v>333</v>
+      </c>
+      <c r="D88" t="s">
+        <v>334</v>
+      </c>
+      <c r="E88" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" t="s">
+        <v>336</v>
+      </c>
+      <c r="D89" t="s">
+        <v>337</v>
+      </c>
+      <c r="E89" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>338</v>
+      </c>
+      <c r="B90" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90" t="s">
+        <v>339</v>
+      </c>
+      <c r="D90" t="s">
+        <v>340</v>
+      </c>
+      <c r="E90" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91" t="s">
+        <v>342</v>
+      </c>
+      <c r="D91" t="s">
+        <v>367</v>
+      </c>
+      <c r="E91" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>343</v>
+      </c>
+      <c r="B92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" t="s">
+        <v>344</v>
+      </c>
+      <c r="D92" t="s">
+        <v>345</v>
+      </c>
+      <c r="E92" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2963,9 +3806,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>100</v>
       </c>
@@ -2977,7 +3820,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>105</v>
       </c>
@@ -2989,7 +3832,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>109</v>
       </c>
@@ -3001,7 +3844,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>113</v>
       </c>
@@ -3013,7 +3856,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>117</v>
       </c>
@@ -3025,7 +3868,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -3037,7 +3880,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
@@ -3049,7 +3892,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>129</v>
       </c>
@@ -3061,7 +3904,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>133</v>
       </c>
@@ -3073,7 +3916,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>165</v>
       </c>
@@ -3085,7 +3928,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>169</v>
       </c>
@@ -3097,7 +3940,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>173</v>
       </c>
@@ -3109,7 +3952,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>177</v>
       </c>
@@ -3121,7 +3964,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>137</v>
       </c>
@@ -3133,7 +3976,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>141</v>
       </c>
@@ -3145,7 +3988,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>181</v>
       </c>
@@ -3157,43 +4000,43 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>237</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A17,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A18,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A19,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
@@ -3205,7 +4048,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
@@ -3217,19 +4060,19 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A22,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v>NODE NOT FOUND</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -3241,19 +4084,19 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C24" t="str" cm="1">
         <f t="array" ref="C24">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A24,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v>NODE NOT FOUND</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
@@ -3265,7 +4108,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
@@ -3277,7 +4120,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -3289,7 +4132,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
@@ -3301,7 +4144,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
@@ -3313,7 +4156,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
@@ -3325,7 +4168,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>47</v>
       </c>
@@ -3337,7 +4180,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>51</v>
       </c>
@@ -3349,7 +4192,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>55</v>
       </c>
@@ -3361,7 +4204,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -3373,7 +4216,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>86</v>
       </c>
@@ -3385,7 +4228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>88</v>
       </c>
@@ -3397,7 +4240,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>63</v>
       </c>
@@ -3409,7 +4252,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
@@ -3421,7 +4264,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
         <v>71</v>
       </c>
@@ -3433,7 +4276,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>75</v>
       </c>
@@ -3445,7 +4288,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>79</v>
       </c>
@@ -3457,7 +4300,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>82</v>
       </c>
@@ -3469,19 +4312,19 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C43" t="str" cm="1">
         <f t="array" ref="C43">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A43,Sheet!$A$2:$A$8004,1,FALSE))</f>
         <v>NODE NOT FOUND</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>92</v>
       </c>
@@ -3493,7 +4336,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
         <v>96</v>
       </c>

</xml_diff>